<commit_message>
GEOME fields with mapping to draft iSamples (in -config.json)
</commit_message>
<xml_diff>
--- a/background/GEOME-MeyerBiocubeTemplateFields.xlsx
+++ b/background/GEOME-MeyerBiocubeTemplateFields.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\iSamples\metadata\background\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{57495E1A-9744-4BC9-809D-38E3D39D5790}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0839FFEF-413F-4106-840A-3192B555ACAE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1050" yWindow="870" windowWidth="26175" windowHeight="14550" tabRatio="715" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1050" yWindow="870" windowWidth="17940" windowHeight="14550" tabRatio="715" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,18 @@
     <sheet name="event_photos_Fields" sheetId="9" r:id="rId9"/>
     <sheet name="Lists" sheetId="10" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -7926,7 +7937,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>

</xml_diff>